<commit_message>
Artefatos 15 - 20
</commit_message>
<xml_diff>
--- a/Artefatos/17 - Análise dos Eventos para cada Cenário.xlsx
+++ b/Artefatos/17 - Análise dos Eventos para cada Cenário.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e90e968d6f8cb6a5/Documentos/^N Faculdade/OPE/smart-owl/Artefatos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e90e968d6f8cb6a5/Documentos/^N Faculdade/3º Semestre/ER/[SI3B] ER ACs/AC 04 ER/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="13_ncr:1_{018EFCCD-0957-454A-8321-5F27ADF1958F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1963C827-0785-44C3-8EDA-2B1EE38CFD7E}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="13_ncr:1_{018EFCCD-0957-454A-8321-5F27ADF1958F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{055D3F6F-F5A6-4C03-A8D5-36C377592A2A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t xml:space="preserve">Externo </t>
   </si>
@@ -84,9 +84,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>x (5)</t>
-  </si>
-  <si>
     <t>x (6)</t>
   </si>
   <si>
@@ -99,12 +96,6 @@
     <t>Candidato entrega protocolo de inscrição e documentos</t>
   </si>
   <si>
-    <t>x (10)</t>
-  </si>
-  <si>
-    <t>x (12)</t>
-  </si>
-  <si>
     <t> Fornecer Resultado de Processo Seletivo</t>
   </si>
   <si>
@@ -138,13 +129,25 @@
     <t>Candidato não solicita resultado</t>
   </si>
   <si>
-    <t>x (10, 11)</t>
-  </si>
-  <si>
     <t>Candidato solicita efetivação de matrícula</t>
   </si>
   <si>
     <t>Candidato devolve prova preenchida</t>
+  </si>
+  <si>
+    <t>Pedagógico entrega prova para confecção</t>
+  </si>
+  <si>
+    <t>x (9)</t>
+  </si>
+  <si>
+    <t>x (11)</t>
+  </si>
+  <si>
+    <t>x (11, 12)</t>
+  </si>
+  <si>
+    <t>x (13)</t>
   </si>
 </sst>
 </file>
@@ -245,7 +248,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -268,11 +271,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -301,9 +341,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -357,13 +394,28 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -711,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,22 +784,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="9" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" s="9" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="25"/>
       <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
@@ -774,10 +826,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="2">
@@ -786,38 +838,38 @@
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21" t="s">
+      <c r="E3" s="20"/>
+      <c r="F3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="23"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="22"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="2">
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23" t="s">
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="3">
@@ -826,298 +878,316 @@
       <c r="D5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11" t="s">
+      <c r="E5" s="10"/>
+      <c r="F5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="27"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="3">
         <v>4</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="2">
+        <v>6</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="3">
+        <v>7</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3">
+        <v>8</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="2">
+        <v>9</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="2">
+        <v>10</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="25" t="s">
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="10">
-        <v>5</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="10">
-        <v>6</v>
-      </c>
-      <c r="D8" s="14" t="s">
+      <c r="C13" s="3">
+        <v>11</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3">
+        <v>12</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2">
+        <v>13</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="10">
-        <v>7</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="13"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="10">
-        <v>8</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="10">
-        <v>9</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="13"/>
-    </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="2">
+        <v>14</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="16">
-        <v>10</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="16">
-        <v>11</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13" s="13"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="10">
-        <v>12</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="13"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="10">
-        <v>13</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="13"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
+      <c r="E16" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+      <c r="A17" s="14"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+      <c r="A18" s="14"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="G19"/>
-      <c r="K19" s="17"/>
+      <c r="A19" s="14"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
       <c r="G20"/>
-      <c r="K20" s="17"/>
+      <c r="K20" s="16"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="17"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
       <c r="G21"/>
-      <c r="K21" s="17"/>
+      <c r="K21" s="16"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="17"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="16"/>
       <c r="G22"/>
-      <c r="K22" s="17"/>
+      <c r="K22" s="16"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="17"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="16"/>
       <c r="G23"/>
-      <c r="K23" s="17"/>
+      <c r="K23" s="16"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="17"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="16"/>
       <c r="G24"/>
-      <c r="K24" s="17"/>
+      <c r="K24" s="16"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="17"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="16"/>
       <c r="G25"/>
-      <c r="K25" s="17"/>
+      <c r="K25" s="16"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="16"/>
       <c r="G26"/>
-      <c r="K26" s="17"/>
+      <c r="K26" s="16"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
       <c r="G27"/>
-      <c r="K27" s="17"/>
+      <c r="K27" s="16"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="G28"/>
+      <c r="K28" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="B3:B4"/>
@@ -1125,11 +1195,11 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>